<commit_message>
front end v1 done
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
   <si>
     <t xml:space="preserve">SI No</t>
   </si>
   <si>
+    <t xml:space="preserve">Registration No</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Computer Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THAUSCS027</t>
   </si>
   <si>
     <t xml:space="preserve">AJ</t>
@@ -177,15 +183,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,27 +217,33 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>42</v>
       </c>
     </row>
@@ -239,21 +252,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -262,21 +278,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>20</v>
       </c>
     </row>
@@ -285,21 +304,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -308,21 +330,24 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>18</v>
       </c>
     </row>
@@ -331,21 +356,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -354,21 +382,24 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -377,21 +408,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>20</v>
       </c>
     </row>
@@ -400,21 +434,24 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -423,21 +460,24 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>18</v>
       </c>
     </row>
@@ -446,21 +486,24 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>32</v>
       </c>
     </row>
@@ -469,21 +512,24 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -492,21 +538,24 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>20</v>
       </c>
     </row>
@@ -515,21 +564,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -538,21 +590,24 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>